<commit_message>
txt und initial Excel
</commit_message>
<xml_diff>
--- a/Stability Metric.xlsx
+++ b/Stability Metric.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klaus/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klaus/GitHub/LEANres/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -783,7 +783,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7541,11 +7540,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142691408"/>
-        <c:axId val="-2113782016"/>
+        <c:axId val="-2134302352"/>
+        <c:axId val="-2109355184"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="2142691408"/>
+        <c:axId val="-2134302352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7588,14 +7587,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2113782016"/>
+        <c:crossAx val="-2109355184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2113782016"/>
+        <c:axId val="-2109355184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7646,7 +7645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142691408"/>
+        <c:crossAx val="-2134302352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7660,7 +7659,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7767,7 +7765,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8495,11 +8492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2100452144"/>
-        <c:axId val="2143596656"/>
+        <c:axId val="-2127984912"/>
+        <c:axId val="-2107671408"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="-2100452144"/>
+        <c:axId val="-2127984912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8542,14 +8539,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2143596656"/>
+        <c:crossAx val="-2107671408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2143596656"/>
+        <c:axId val="-2107671408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8600,7 +8597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2100452144"/>
+        <c:crossAx val="-2127984912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8614,7 +8611,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8726,7 +8722,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10570,11 +10565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090656160"/>
-        <c:axId val="-2071698592"/>
+        <c:axId val="-2099791888"/>
+        <c:axId val="-2135681280"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="-2090656160"/>
+        <c:axId val="-2099791888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10617,14 +10612,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071698592"/>
+        <c:crossAx val="-2135681280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2071698592"/>
+        <c:axId val="-2135681280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10674,7 +10669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090656160"/>
+        <c:crossAx val="-2099791888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10688,7 +10683,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10800,7 +10794,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14282,11 +14275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090212320"/>
-        <c:axId val="-2090391376"/>
+        <c:axId val="-2126718000"/>
+        <c:axId val="-2102103504"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="-2090212320"/>
+        <c:axId val="-2126718000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14329,14 +14322,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090391376"/>
+        <c:crossAx val="-2102103504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2090391376"/>
+        <c:axId val="-2102103504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14387,7 +14380,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090212320"/>
+        <c:crossAx val="-2126718000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14401,7 +14394,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14483,7 +14475,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15013,11 +15004,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109331296"/>
-        <c:axId val="-2071220800"/>
+        <c:axId val="-2122234864"/>
+        <c:axId val="-2128054272"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="2109331296"/>
+        <c:axId val="-2122234864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15060,14 +15051,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071220800"/>
+        <c:crossAx val="-2128054272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2071220800"/>
+        <c:axId val="-2128054272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15118,7 +15109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109331296"/>
+        <c:crossAx val="-2122234864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15132,7 +15123,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -18072,11 +18062,11 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="1"/>
-            <a:t>What is this spreadsheet</a:t>
+            <a:t>What is this </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
-            <a:t> for?</a:t>
+            <a:t>for?</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -21444,7 +21434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -21478,7 +21468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -21507,9 +21497,7 @@
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
-        <v>41085</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>41085</v>
       </c>

</xml_diff>